<commit_message>
Se modifica secuencial y se agrega funcion (libreria)
</commit_message>
<xml_diff>
--- a/Parcial 2/datosVerificacionAlgoritmo.xlsx
+++ b/Parcial 2/datosVerificacionAlgoritmo.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>y</t>
   </si>
@@ -133,12 +133,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -421,10 +424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J38"/>
+  <dimension ref="A1:U38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -437,15 +440,19 @@
     <col min="6" max="6" width="4.7109375" style="1" customWidth="1"/>
     <col min="7" max="7" width="5" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="11.42578125" style="1"/>
+    <col min="9" max="12" width="11.42578125" style="1"/>
+    <col min="13" max="15" width="2" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.42578125" style="1"/>
+    <col min="17" max="21" width="2" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="E1" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -456,7 +463,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -467,7 +474,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
@@ -498,8 +505,23 @@
       <c r="J5" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="Q5" s="3">
+        <v>6</v>
+      </c>
+      <c r="R5" s="3">
+        <v>5</v>
+      </c>
+      <c r="S5" s="3">
+        <v>6</v>
+      </c>
+      <c r="T5" s="3">
+        <v>3</v>
+      </c>
+      <c r="U5" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>0</v>
       </c>
@@ -525,8 +547,23 @@
         <f>A6*5+B6</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="Q6" s="3">
+        <v>4</v>
+      </c>
+      <c r="R6" s="3">
+        <v>5</v>
+      </c>
+      <c r="S6" s="3">
+        <v>6</v>
+      </c>
+      <c r="T6" s="3">
+        <v>3</v>
+      </c>
+      <c r="U6" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>0</v>
       </c>
@@ -552,8 +589,32 @@
         <f>A7*5+B7</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M7" s="3">
+        <v>2</v>
+      </c>
+      <c r="N7" s="3">
+        <v>3</v>
+      </c>
+      <c r="O7" s="3">
+        <v>4</v>
+      </c>
+      <c r="Q7" s="3">
+        <v>2</v>
+      </c>
+      <c r="R7" s="3">
+        <v>2</v>
+      </c>
+      <c r="S7" s="3">
+        <v>5</v>
+      </c>
+      <c r="T7" s="3">
+        <v>1</v>
+      </c>
+      <c r="U7" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>0</v>
       </c>
@@ -579,8 +640,32 @@
         <f t="shared" ref="H8:H38" si="0">A8*5+B8</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M8" s="3">
+        <v>5</v>
+      </c>
+      <c r="N8" s="3">
+        <v>1</v>
+      </c>
+      <c r="O8" s="3">
+        <v>5</v>
+      </c>
+      <c r="Q8" s="3">
+        <v>2</v>
+      </c>
+      <c r="R8" s="3">
+        <v>5</v>
+      </c>
+      <c r="S8" s="3">
+        <v>9</v>
+      </c>
+      <c r="T8" s="3">
+        <v>3</v>
+      </c>
+      <c r="U8" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>0</v>
       </c>
@@ -606,8 +691,32 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M9" s="3">
+        <v>6</v>
+      </c>
+      <c r="N9" s="3">
+        <v>2</v>
+      </c>
+      <c r="O9" s="3">
+        <v>6</v>
+      </c>
+      <c r="Q9" s="3">
+        <v>1</v>
+      </c>
+      <c r="R9" s="3">
+        <v>5</v>
+      </c>
+      <c r="S9" s="3">
+        <v>6</v>
+      </c>
+      <c r="T9" s="3">
+        <v>3</v>
+      </c>
+      <c r="U9" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>0</v>
       </c>
@@ -634,7 +743,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>1</v>
       </c>
@@ -661,7 +770,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>1</v>
       </c>
@@ -694,8 +803,14 @@
         <f>E12*5+F12+(B12-A12)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M12" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>1</v>
       </c>
@@ -729,7 +844,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>1</v>
       </c>
@@ -763,7 +878,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>1</v>
       </c>
@@ -797,7 +912,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>1</v>
       </c>

</xml_diff>